<commit_message>
VSM, Tecnomatix final y celda 1
</commit_message>
<xml_diff>
--- a/project/Documents/03. KPIs.xlsx
+++ b/project/Documents/03. KPIs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yovan\Desktop\APM\ausol-apm.github.io\project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB66A737-6E5A-49D3-AD54-C66DCFF6F2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3334B3F-6703-4750-B414-8807AF66BF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempos" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="144">
   <si>
     <t>Etapa</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Control de calidad</t>
   </si>
   <si>
-    <t>Calcomanias</t>
-  </si>
-  <si>
     <t>Empaquetado</t>
   </si>
   <si>
@@ -149,15 +146,6 @@
     <t>Buffers a bufferAssembler</t>
   </si>
   <si>
-    <t>Assembler a calidad</t>
-  </si>
-  <si>
-    <t>Calidad a calcomanias</t>
-  </si>
-  <si>
-    <t>calcomanias a empaquetado</t>
-  </si>
-  <si>
     <t>Unidades por tanda</t>
   </si>
   <si>
@@ -251,15 +239,6 @@
     <t>Tiempo entre turnos</t>
   </si>
   <si>
-    <t>PENDIENTE WIP - VSM</t>
-  </si>
-  <si>
-    <t>Unidades tanda</t>
-  </si>
-  <si>
-    <t>Takt</t>
-  </si>
-  <si>
     <t>Jornada (h)</t>
   </si>
   <si>
@@ -299,9 +278,6 @@
     <t>TER (h)</t>
   </si>
   <si>
-    <t>TANP (h)</t>
-  </si>
-  <si>
     <t>PE</t>
   </si>
   <si>
@@ -314,18 +290,12 @@
     <t>Q</t>
   </si>
   <si>
-    <t>Se tiene un desfase del 10% en los tiempos y producción real</t>
-  </si>
-  <si>
     <t>Acabado</t>
   </si>
   <si>
     <t>Tandas por lote</t>
   </si>
   <si>
-    <t>Estación</t>
-  </si>
-  <si>
     <t>Separar</t>
   </si>
   <si>
@@ -341,28 +311,166 @@
     <t>Relación transporte</t>
   </si>
   <si>
-    <t>6 a a7</t>
-  </si>
-  <si>
-    <t>0 a 1</t>
-  </si>
-  <si>
-    <t>Tp (h)</t>
-  </si>
-  <si>
-    <t>Tt (h)</t>
-  </si>
-  <si>
     <t>Los tiempos en el VSM son por tanda… Ya que es una tarea dispendiosa, hacerlo por unidad</t>
   </si>
   <si>
-    <t>Relación proceso</t>
-  </si>
-  <si>
     <t>No es posible encontrar la relación real entre las inyectoras y los moldes de manera directa. Entonces, se parte de los resultados de Tecnomatix, para la obtención de esos tiempos, partiendo de un la suma los productos sobre el tiempo requerido para su producción</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Tampografía</t>
+  </si>
+  <si>
+    <t>Assembler a tampografía</t>
+  </si>
+  <si>
+    <t>Tampografía a calidad</t>
+  </si>
+  <si>
+    <t>Calidad a empaquetado</t>
+  </si>
+  <si>
+    <t>Valor en pelletSource</t>
+  </si>
+  <si>
+    <t>Takt (s)</t>
+  </si>
+  <si>
+    <t>TINP (h)</t>
+  </si>
+  <si>
+    <t>Se asume un desfase del 10% en los tiempos y producción real, los calculos previos ya tienen incorporado el 3% en defectuosos</t>
+  </si>
+  <si>
+    <t>Piezas moto</t>
+  </si>
+  <si>
+    <t>Cantidad por tanda</t>
+  </si>
+  <si>
+    <t>Juguete</t>
+  </si>
+  <si>
+    <t>Moto</t>
+  </si>
+  <si>
+    <t>Barco</t>
+  </si>
+  <si>
+    <t>Casa</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Rueda</t>
+  </si>
+  <si>
+    <t>Chasis</t>
+  </si>
+  <si>
+    <t>Piezas Barco</t>
+  </si>
+  <si>
+    <t>Timon 1</t>
+  </si>
+  <si>
+    <t>Timon 2</t>
+  </si>
+  <si>
+    <t>Superior</t>
+  </si>
+  <si>
+    <t>Inferior</t>
+  </si>
+  <si>
+    <t>Por tanda</t>
+  </si>
+  <si>
+    <t>Piezas Casa</t>
+  </si>
+  <si>
+    <t>Paredes</t>
+  </si>
+  <si>
+    <t>Puerta</t>
+  </si>
+  <si>
+    <t>Techo</t>
+  </si>
+  <si>
+    <t>Moldes por tanda</t>
+  </si>
+  <si>
+    <t>Empaquetado a caja</t>
+  </si>
+  <si>
+    <t>Proceso</t>
+  </si>
+  <si>
+    <t>Inyectora a separación</t>
+  </si>
+  <si>
+    <t>Separación a acabados</t>
+  </si>
+  <si>
+    <t>Acabados a ensamble</t>
+  </si>
+  <si>
+    <t>Ensamble a pintura</t>
+  </si>
+  <si>
+    <t>Pintura a calidad</t>
+  </si>
+  <si>
+    <t>Cajas a robot</t>
+  </si>
+  <si>
+    <t>Tiempo total por tanda (s)</t>
+  </si>
+  <si>
+    <t>Tiempo medio (s)</t>
+  </si>
+  <si>
+    <t>Robot a despacho</t>
+  </si>
+  <si>
+    <t>Total tiempo</t>
+  </si>
+  <si>
+    <t>Total (h)</t>
+  </si>
+  <si>
+    <t>Tp (s)</t>
+  </si>
+  <si>
+    <t>Tandas reales (tandas/dia)</t>
+  </si>
+  <si>
+    <t>Por día (s)</t>
+  </si>
+  <si>
+    <t>Día (h)</t>
+  </si>
+  <si>
+    <t>Total (s)</t>
+  </si>
+  <si>
+    <t>Juguetes por caja</t>
+  </si>
+  <si>
+    <t>Cajas por pallet</t>
+  </si>
+  <si>
+    <t>Unidades por dia</t>
+  </si>
+  <si>
+    <t>Total cajas (día)</t>
+  </si>
+  <si>
+    <t>Total pallets (día)</t>
   </si>
 </sst>
 </file>
@@ -373,7 +481,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,8 +512,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,8 +540,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor theme="7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -433,12 +573,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -461,30 +645,72 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -496,18 +722,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -521,6 +750,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -595,7 +829,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
+      <xdr:colOff>635000</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>162013</xdr:rowOff>
     </xdr:to>
@@ -633,15 +867,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1485901</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>117903</xdr:rowOff>
+      <xdr:colOff>2044701</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>73453</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1136651</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>139907</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>482601</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95457</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -664,7 +898,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3854451" y="2143553"/>
+          <a:off x="4552951" y="1914953"/>
           <a:ext cx="3276600" cy="758604"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -677,15 +911,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>174933</xdr:rowOff>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>92383</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>283924</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>146283</xdr:rowOff>
+      <xdr:colOff>322024</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63733</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -708,7 +942,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6991350" y="1279833"/>
+          <a:off x="7607300" y="1381433"/>
           <a:ext cx="3020774" cy="523800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -720,16 +954,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>138807</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>30857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>312549</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>133611</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>553849</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>25661</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -752,7 +986,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7772400" y="2532757"/>
+          <a:off x="4686300" y="3529707"/>
           <a:ext cx="3925699" cy="731404"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -764,16 +998,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1943100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>147295</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>429892</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1109342</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>117954</xdr:rowOff>
+      <xdr:rowOff>168754</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -781,6 +1015,230 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DD559EF-9011-9EB5-75BD-A2C9BD4FAC3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect t="35691"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="292100" y="3962400"/>
+          <a:ext cx="3325492" cy="810104"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>130917</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>111439</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7E52C5-BF86-DC06-DB4F-C438C5C7DC71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2524867"/>
+          <a:ext cx="3543300" cy="1269572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>53109</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>61097</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03DD5D32-88F9-0E81-AD50-DCED44275BDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8591550" y="53109"/>
+          <a:ext cx="3136900" cy="928738"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>13852</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>753208</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>57442</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E8E81E2-3142-7205-9593-F43065456F9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8267700" y="1302902"/>
+          <a:ext cx="3337658" cy="1332640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>33901</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>404277</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>54269</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C63D3C0D-51F1-9492-8533-CA1853032D54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5492750" y="2059551"/>
+          <a:ext cx="2709327" cy="756968"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>22675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123965</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95AA463E-68E1-DBAE-54F8-CE215954866D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -796,8 +1254,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4140200" y="3461995"/>
-          <a:ext cx="3325492" cy="1259709"/>
+          <a:off x="2914650" y="1864175"/>
+          <a:ext cx="2374900" cy="1206190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -810,7 +1268,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E18C99A6-A7D5-417D-A109-187311EB94FC}" name="Tabla1" displayName="Tabla1" ref="A2:E17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E18C99A6-A7D5-417D-A109-187311EB94FC}" name="Tabla1" displayName="Tabla1" ref="A2:E17" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A2:E17" xr:uid="{E18C99A6-A7D5-417D-A109-187311EB94FC}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -822,11 +1280,11 @@
     <sortCondition ref="A2:A16"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{19CD4D76-1CC5-48BF-9617-AC7EBCBF03D9}" name="N°" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{060C4D4C-E2DC-4A58-8261-94F68CD86310}" name="Etapa" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{F5886262-8B66-44DE-A8CA-CCD44FAC65B8}" name="Proceso (s)" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{62AD91F2-5982-477A-8D8D-CF99BCF1C482}" name="Set-up (s)" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{E66446FC-83A2-4C34-BC92-FE1238C0EFCC}" name="Total" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{19CD4D76-1CC5-48BF-9617-AC7EBCBF03D9}" name="N°" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{060C4D4C-E2DC-4A58-8261-94F68CD86310}" name="Etapa" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{F5886262-8B66-44DE-A8CA-CCD44FAC65B8}" name="Proceso (s)" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{62AD91F2-5982-477A-8D8D-CF99BCF1C482}" name="Set-up (s)" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{E66446FC-83A2-4C34-BC92-FE1238C0EFCC}" name="Total" dataDxfId="15">
       <calculatedColumnFormula>C3+D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -835,41 +1293,48 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BC58768C-2D7E-4818-B4AA-BDD95BDEC2CD}" name="Tabla13" displayName="Tabla13" ref="A20:D31" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A20:D31" xr:uid="{BC58768C-2D7E-4818-B4AA-BDD95BDEC2CD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:D31">
-    <sortCondition ref="A20:A31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BC58768C-2D7E-4818-B4AA-BDD95BDEC2CD}" name="Tabla13" displayName="Tabla13" ref="A20:D32" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A20:D32" xr:uid="{BC58768C-2D7E-4818-B4AA-BDD95BDEC2CD}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:D32">
+    <sortCondition ref="A20:A32"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2E55E79A-A296-47B0-B232-9DFF752231C2}" name="N°" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{E7AA5353-4CAE-4333-85DE-D237E1BC7118}" name="Ubicación" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{CD0B87CE-1351-44F6-9ACE-B3E8564515ED}" name="Tiempo" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{CDF80DF5-5F66-4BE8-9877-EFFB1C20A674}" name="Descripción detallada" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{2E55E79A-A296-47B0-B232-9DFF752231C2}" name="N°" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{E7AA5353-4CAE-4333-85DE-D237E1BC7118}" name="Ubicación" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{CD0B87CE-1351-44F6-9ACE-B3E8564515ED}" name="Tiempo" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{CDF80DF5-5F66-4BE8-9877-EFFB1C20A674}" name="Descripción detallada" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1E7802E5-DEBF-4605-AC7B-EFF1F76CF9FB}" name="Tabla4" displayName="Tabla4" ref="A1:D10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:D10" xr:uid="{1E7802E5-DEBF-4605-AC7B-EFF1F76CF9FB}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1E7802E5-DEBF-4605-AC7B-EFF1F76CF9FB}" name="Tabla4" displayName="Tabla4" ref="B15:D24" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B15:D24" xr:uid="{1E7802E5-DEBF-4605-AC7B-EFF1F76CF9FB}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DD8BD99A-55EB-43B2-85C0-40D72F09E04F}" name="Estación" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{C3DCC130-017E-4F1E-92EB-E315A1AEBA87}" name="Tp (h)" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{624EB0B8-1FBC-496F-AEB6-4797A4A5FC89}" name="Transporte" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{A44E6FD6-1AF4-42AB-A3FE-3BCC3A03A411}" name="Tt (h)" dataDxfId="2"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DD8BD99A-55EB-43B2-85C0-40D72F09E04F}" name="Proceso" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C3DCC130-017E-4F1E-92EB-E315A1AEBA87}" name="Tp (s)" dataDxfId="5">
+      <calculatedColumnFormula>Tiempos!E5*VSM!$G$7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{F2156E13-D132-4894-A3B0-34414D91D3A9}" name="Día (h)" dataDxfId="4">
+      <calculatedColumnFormula>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B029FE5-C33B-4E02-A4C8-0A378815E268}" name="Tabla3" displayName="Tabla3" ref="A2:J5" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B029FE5-C33B-4E02-A4C8-0A378815E268}" name="Tabla3" displayName="Tabla3" ref="A2:J5" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A2:J5" xr:uid="{5B029FE5-C33B-4E02-A4C8-0A378815E268}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -883,13 +1348,13 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{FD3036A3-92C4-47AD-AEAD-4738A5E2A4E3}" name="Indicadores" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FD3036A3-92C4-47AD-AEAD-4738A5E2A4E3}" name="Indicadores" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{45921F43-9ADF-496E-9A01-4F8D3E6BB354}" name="Inyección"/>
     <tableColumn id="3" xr3:uid="{CD10CB41-58D2-422E-98F4-84460853D09E}" name="Separado"/>
     <tableColumn id="4" xr3:uid="{304B0503-DEFE-4B0F-A316-C8BCC301392D}" name="Acabado"/>
     <tableColumn id="6" xr3:uid="{1369ADB9-7C04-46C0-8463-92CC60AD6ED2}" name="Ensamble general"/>
-    <tableColumn id="7" xr3:uid="{74D6D253-8C91-4922-A738-A64961372299}" name="Calidad"/>
-    <tableColumn id="5" xr3:uid="{DF0B388F-BE48-4DC1-9DFA-156D535A63E3}" name="Calcomanias"/>
+    <tableColumn id="7" xr3:uid="{74D6D253-8C91-4922-A738-A64961372299}" name="Tampografía" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{DF0B388F-BE48-4DC1-9DFA-156D535A63E3}" name="Calidad" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{A6F638C7-33A8-4B22-8E0B-18452822789D}" name="Empaquetado"/>
     <tableColumn id="9" xr3:uid="{108E8E86-038E-46DE-B6EC-0298F9BA78D8}" name="Palletizado"/>
     <tableColumn id="10" xr3:uid="{B6D79683-564E-46DA-BB68-BAC4B4264CC9}" name="Despacho"/>
@@ -1161,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32872503-A03D-4A72-A530-385213610AD9}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1174,27 +1639,25 @@
     <col min="3" max="3" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.90625" style="1"/>
+    <col min="6" max="6" width="20.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-    </row>
-    <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1208,74 +1671,74 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="19"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1">
         <f>C3+D3</f>
-        <v>85</v>
-      </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1.2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" ref="E4:E5" si="0">C4+D4</f>
-        <v>85</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1.3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1283,20 +1746,19 @@
         <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6:E17" si="1">C6+D6</f>
-        <v>90</v>
-      </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1304,19 +1766,19 @@
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>3.1</v>
       </c>
@@ -1333,10 +1795,10 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>3.2</v>
       </c>
@@ -1353,10 +1815,9 @@
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>4.0999999999999996</v>
       </c>
@@ -1367,16 +1828,15 @@
         <v>2</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>4.2</v>
       </c>
@@ -1387,16 +1847,15 @@
         <v>2.5</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3.5</v>
+      </c>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>4.3</v>
       </c>
@@ -1407,321 +1866,316 @@
         <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <f>C13+D13</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
         <v>5</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <v>5</v>
       </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <f>C14+D14</f>
         <v>6</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>5.03</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>5.03</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="1"/>
-        <v>5.03</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>10.06</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D17" s="1">
         <v>10</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1">
         <f>SUM(Tabla1[Total])</f>
-        <v>412.03</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>221.06</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="13">
-        <f>E18/SUM($E$18,$C$32)</f>
-        <v>0.69950596743799121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1.2</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1">
         <v>20</v>
       </c>
-      <c r="C22" s="1">
-        <v>30</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" t="s">
-        <v>99</v>
-      </c>
-      <c r="G22" s="13">
-        <f>C32/SUM($E$18,$C$32)</f>
-        <v>0.30049403256200874</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>2.1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="4">
+        <v>20</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>3.1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>3.2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="4">
         <v>2</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>5</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="4">
         <v>15</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C31" s="1">
         <v>2</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="4">
-        <v>8</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="4">
-        <v>12</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B32" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="4">
+        <v>9</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="4">
         <v>14</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="1">
         <f>SUM(Tabla13[Tiempo])</f>
-        <v>177</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="A19:D19"/>
-    <mergeCell ref="F19:H19"/>
     <mergeCell ref="G2:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1735,204 +2189,635 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50DB93E-6A43-49FD-BECD-E21C2093DF0D}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.81640625" customWidth="1"/>
+    <col min="9" max="9" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.36328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.90625" style="37"/>
+    <col min="14" max="14" width="7.90625" customWidth="1"/>
+    <col min="15" max="15" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B2" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="22">
+        <f>$G$2*B2</f>
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="1">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1">
+        <f>AVERAGE(Tiempos!C21:C22)</f>
+        <v>15</v>
+      </c>
+      <c r="K2" s="22">
+        <f>J2*$G$7</f>
+        <v>45</v>
+      </c>
+      <c r="L2" s="35">
+        <f>K2*'P. Rendimiento'!$B$1/3600</f>
+        <v>1.1875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="22">
+        <f>$G$2*B3</f>
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="1">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J3" s="1">
+        <f>AVERAGE(Tiempos!C23:C24)</f>
+        <v>15</v>
+      </c>
+      <c r="K3" s="22">
+        <f>J3*$C$13/40</f>
+        <v>36.75</v>
+      </c>
+      <c r="L3" s="35">
+        <f>K3*'P. Rendimiento'!$B$1/3600</f>
+        <v>0.96979166666666672</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" s="1">
+        <f>AVERAGE(Tiempos!C25:C27)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="K4" s="22">
+        <f>J4*$C$13/40</f>
+        <v>27.766666666666669</v>
+      </c>
+      <c r="L4" s="35">
+        <f>K4*'P. Rendimiento'!$B$1/3600</f>
+        <v>0.73273148148148148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="22">
+        <f>$G$3*B5</f>
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="22">
+        <f>SUM(G2:G4)</f>
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J5" s="1">
+        <f>Tiempos!C28</f>
+        <v>15</v>
+      </c>
+      <c r="K5" s="22">
+        <f>J5*$G$5/$G$5</f>
+        <v>15</v>
+      </c>
+      <c r="L5" s="35">
+        <f>K5*'P. Rendimiento'!$B$1/3600</f>
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="22">
+        <f>$G$3*B6</f>
+        <v>7</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" s="1">
+        <f>Tiempos!C29</f>
+        <v>10</v>
+      </c>
+      <c r="K6" s="22">
+        <f>J6*$G$5/$G$5</f>
+        <v>10</v>
+      </c>
+      <c r="L6" s="35">
+        <f>K6*'P. Rendimiento'!$B$1/3600</f>
+        <v>0.2638888888888889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="22">
+        <f>$G$3*B7</f>
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="1">
+        <f>Tiempos!C30</f>
+        <v>4</v>
+      </c>
+      <c r="K7" s="22">
+        <f>J7*$G$5</f>
+        <v>80</v>
+      </c>
+      <c r="L7" s="35">
+        <f>K7*'P. Rendimiento'!$B$1/3600</f>
+        <v>2.1111111111111112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="22">
+        <f>$G$3*B8</f>
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8" s="1">
+        <f>Tiempos!C32</f>
+        <v>14</v>
+      </c>
+      <c r="K8" s="22">
+        <f>L8*3600/'P. Rendimiento'!B1</f>
+        <v>11.2</v>
+      </c>
+      <c r="L8" s="36">
+        <f>J8*G11/3600</f>
+        <v>0.29555555555555557</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G9" s="22">
+        <v>25</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="22">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K9" s="27">
+        <v>0</v>
+      </c>
+      <c r="L9" s="35">
+        <f>K9*'P. Rendimiento'!$B$1/3600</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <f>B10*$G$4</f>
+        <v>20</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" s="22">
+        <v>20</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K10" s="22">
+        <f>SUM(K2:K9)</f>
+        <v>225.71666666666664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <f>B11*$G$4</f>
+        <v>5</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="22">
+        <f>'P. Rendimiento'!$F$5/VSM!G9</f>
+        <v>76</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="L11" s="37">
+        <f>SUM(L2:L9)</f>
+        <v>5.9564120370370368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <f>B12*$G$4</f>
+        <v>5</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="22">
+        <f>G11/G10</f>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1">
+        <f>SUM(C2:C3)+SUM(C5:C8)+SUM(C10:C12)</f>
         <v>98</v>
       </c>
-      <c r="G2" s="13">
-        <f>B11/SUM($B$11,$D$11)</f>
-        <v>0.85722195229431786</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="1">
-        <v>11.88</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="11">
+        <f>C25/G17</f>
+        <v>0.81325635794328555</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15"/>
+      <c r="K15"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="24">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="1">
+        <f>Tiempos!E5*VSM!$G$7</f>
+        <v>120</v>
+      </c>
+      <c r="D16" s="5">
+        <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="11">
+        <f>K10/G17</f>
+        <v>0.18674364205671443</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16"/>
+      <c r="K16"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="24">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="1">
+        <f>Tiempos!E6*VSM!$G$7</f>
+        <v>18</v>
+      </c>
+      <c r="D17" s="5">
+        <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G17" s="28">
+        <f>C25+K10</f>
+        <v>1208.6980000000001</v>
+      </c>
+      <c r="I17" s="22"/>
+      <c r="J17"/>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="24">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G3" s="13">
-        <f>D11/SUM($B$11,$D$11)</f>
-        <v>0.14277804770568212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="1">
-        <v>14.06</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1">
-        <v>3</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="J4" s="14"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="1">
-        <v>6.59</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2.61</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="20"/>
-    </row>
-    <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="1">
-        <v>21.67</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1.96</v>
-      </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="1">
+        <f>Tiempos!E7*$C$13</f>
+        <v>392</v>
+      </c>
+      <c r="D18" s="5">
+        <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
+        <v>10.344444444444445</v>
+      </c>
+      <c r="I18" s="22"/>
+      <c r="J18"/>
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="24">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="1">
+        <f>AVERAGE(Tiempos!E10:E12)*G5</f>
+        <v>63.333333333333329</v>
+      </c>
+      <c r="D19" s="5">
+        <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
+        <v>1.6712962962962961</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="34"/>
+      <c r="I19" s="22"/>
+      <c r="J19"/>
+      <c r="K19"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="24">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="1">
+        <f>Tiempos!E13*G5</f>
+        <v>140</v>
+      </c>
+      <c r="D20" s="5">
+        <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
+        <v>3.6944444444444446</v>
+      </c>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="I20" s="22"/>
+      <c r="J20"/>
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="24">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="1">
+        <f>Tiempos!E14*G5</f>
+        <v>120</v>
+      </c>
+      <c r="D21" s="5">
+        <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="I21" s="22"/>
+      <c r="J21"/>
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="24">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1">
-        <v>8.75</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.96</v>
-      </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1">
-        <v>8.75</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1.05</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0.44444444443999997</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="5">
-        <f>SUM(B2:B10)</f>
-        <v>84.294444444439989</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" ref="D11" si="0">SUM(D2:D10)</f>
-        <v>14.040000000000001</v>
+      <c r="C22" s="1">
+        <f>Tiempos!E15*G5</f>
+        <v>120</v>
+      </c>
+      <c r="D22" s="5">
+        <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="24">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="1">
+        <f>Tiempos!E16*G11/'P. Rendimiento'!B1</f>
+        <v>8.048</v>
+      </c>
+      <c r="D23" s="5">
+        <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
+        <v>0.2123777777777778</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23"/>
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="25">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1">
+        <f>Tiempos!E17*G12/'P. Rendimiento'!B1</f>
+        <v>1.6</v>
+      </c>
+      <c r="D24" s="5">
+        <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
+        <v>4.2222222222222223E-2</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24"/>
+      <c r="K24"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25"/>
+      <c r="B25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="1">
+        <f>SUM(Tabla4[Tp (s)])</f>
+        <v>982.9813333333334</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D26" s="5">
+        <f>SUM(Tabla4[Día (h)])</f>
+        <v>25.939785185185187</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F5:G8"/>
+    <mergeCell ref="F19:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1946,14 +2831,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.90625" style="1" bestFit="1" customWidth="1"/>
@@ -1966,158 +2851,171 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1">
+        <v>95</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="18"/>
+      <c r="D1" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="32"/>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>7</v>
+      <c r="C2" s="5">
+        <f>8 - 70/60</f>
+        <v>6.833333333333333</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1">
         <v>8</v>
       </c>
       <c r="F2" s="1">
         <f>E2*$B$1</f>
-        <v>528</v>
+        <v>760</v>
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G4" si="0">F2*$B$2</f>
-        <v>2640</v>
+        <v>3800</v>
       </c>
       <c r="I2" s="1">
         <f>G2/8</f>
-        <v>330</v>
+        <v>475</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1">
         <f>B2*B1</f>
-        <v>330</v>
-      </c>
-      <c r="C3" s="1">
-        <f>B1*3</f>
-        <v>198</v>
+        <v>475</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1">
         <v>7</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F4" si="1">E3*$B$1</f>
-        <v>462</v>
+        <v>665</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>2310</v>
+        <v>3325</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C4" s="16">
+        <f>(B1*3)</f>
+        <v>285</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1">
         <v>5</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="1"/>
-        <v>330</v>
+        <v>475</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>1650</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="2">
-        <f>C2*60*60/F5</f>
-        <v>19.09090909090909</v>
-      </c>
-      <c r="C5" s="21"/>
+      <c r="A5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="15">
+        <f>C5/3</f>
+        <v>97.850000000000009</v>
+      </c>
+      <c r="C5" s="17">
+        <f>C4*1.03</f>
+        <v>293.55</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>71</v>
+        <v>141</v>
       </c>
       <c r="F5" s="1">
         <f>SUM(F2:F4)</f>
-        <v>1320</v>
-      </c>
-      <c r="G5" s="2">
+        <v>1900</v>
+      </c>
+      <c r="G5" s="20">
         <f>SUM(G2:G4)</f>
-        <v>6600</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>57</v>
+        <v>9500</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G6" s="1">
+        <f>G5*4</f>
+        <v>38000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2">
+        <f>F8*F9*F10*B12</f>
+        <v>9500</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="1">
-        <f>F8*F9*F10*B12</f>
-        <v>6641.5094339622638</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="8">
-        <f>F5/F7</f>
-        <v>0.19875000000000001</v>
+      <c r="I7" s="19">
+        <f>G5/F7</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -2125,17 +3023,17 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B9" s="5">
-        <f>B10/G5</f>
-        <v>0.36136363636363639</v>
+        <f>(C10*C2*60)/G5</f>
+        <v>0.21578947368421053</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F9" s="1">
         <v>5</v>
@@ -2143,69 +3041,73 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B10" s="5">
-        <f>B11*G5</f>
-        <v>2385</v>
+        <f>B9*G5</f>
+        <v>2050</v>
       </c>
       <c r="C10" s="7">
-        <f>B10/60/8</f>
-        <v>4.96875</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1">
-        <v>8</v>
+        <f>C2</f>
+        <v>6.833333333333333</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B11" s="5">
-        <f>60/B12</f>
-        <v>0.36136363636363639</v>
+        <f>B10/G5</f>
+        <v>0.21578947368421053</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="10">
-        <f>F5/(7+(57/60))</f>
-        <v>166.03773584905659</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D17" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="18">
+        <f>60/B11</f>
+        <v>278.04878048780489</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="21">
+        <f>C2*60*60/F5</f>
+        <v>12.947368421052632</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="2">
+        <f>F8*(B8+G5*B9+B21)</f>
+        <v>9730</v>
+      </c>
+      <c r="C20" s="5">
+        <f>B20/60/24</f>
+        <v>6.7569444444444438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1">
+        <f xml:space="preserve"> (16*5 + 48)*60</f>
+        <v>7680</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B20" s="1">
-        <f>F8*(B8+G5*B9+B21)</f>
-        <v>6237</v>
-      </c>
-      <c r="C20" s="1">
-        <f>B20/60/24</f>
-        <v>4.3312499999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="1">
-        <f xml:space="preserve"> 16.05*60*4</f>
-        <v>3852</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2222,8 +3124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B510CC-D191-4B84-AC9A-C3DC17F5F4F7}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2241,68 +3143,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="A1" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1">
-        <f>7*5*4</f>
         <v>140</v>
       </c>
       <c r="C3" s="1">
-        <f>7*5*2</f>
         <v>70</v>
       </c>
       <c r="D3" s="1">
         <v>70</v>
       </c>
       <c r="E3" s="1">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="F3" s="1">
         <v>70</v>
@@ -2322,25 +3222,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="1">
-        <v>3</v>
+      <c r="G4" s="30">
+        <v>1</v>
       </c>
       <c r="H4" s="1">
         <v>3</v>
@@ -2349,154 +3249,160 @@
         <v>8</v>
       </c>
       <c r="J4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="9">
-        <f>B3/SUM(B3:B4)</f>
-        <v>0.92105263157894735</v>
-      </c>
-      <c r="C5" s="9">
-        <f>C3/SUM(C3:C4)</f>
-        <v>0.97222222222222221</v>
-      </c>
-      <c r="D5" s="9">
-        <f>D3/SUM(D3:D4)</f>
-        <v>0.97222222222222221</v>
-      </c>
-      <c r="E5" s="9">
-        <f>E3/SUM(E3:E4)</f>
-        <v>0.89743589743589747</v>
-      </c>
-      <c r="F5" s="9">
-        <f t="shared" ref="F5:J5" si="0">F3/SUM(F3:F4)</f>
-        <v>0.97222222222222221</v>
-      </c>
-      <c r="G5" s="9">
+        <v>69</v>
+      </c>
+      <c r="B5" s="8">
+        <f t="shared" ref="B5:G5" si="0">B3/SUM(B3:B4)</f>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="C5" s="8">
         <f t="shared" si="0"/>
-        <v>0.95890410958904104</v>
-      </c>
-      <c r="H5" s="9">
+        <v>0.9859154929577465</v>
+      </c>
+      <c r="D5" s="8">
         <f t="shared" si="0"/>
-        <v>0.95890410958904104</v>
-      </c>
-      <c r="I5" s="9">
-        <f t="shared" si="0"/>
-        <v>0.94594594594594594</v>
-      </c>
-      <c r="J5" s="9">
+        <v>0.9859154929577465</v>
+      </c>
+      <c r="E5" s="8">
         <f t="shared" si="0"/>
         <v>0.97222222222222221</v>
       </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="G5" s="31">
+        <f t="shared" si="0"/>
+        <v>0.9859154929577465</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" ref="H5:J5" si="1">H3/SUM(H3:H4)</f>
+        <v>0.95890410958904104</v>
+      </c>
+      <c r="I5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.94594594594594594</v>
+      </c>
+      <c r="J5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.9859154929577465</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="9">
+        <f>B8*D8*F8</f>
+        <v>0.87300000000000011</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="14">
+        <f>B9/B10</f>
+        <v>0.99082452574525748</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="8">
+        <f>D9*D10</f>
+        <v>0.90833439889172818</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="10">
-        <f>B8*D8*F8</f>
-        <v>0.99147857142857165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="F8" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+    </row>
+    <row r="9" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="5">
+        <f>B10-B11</f>
+        <v>6.7706342592592588</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="8">
+        <f>('P. Rendimiento'!F5*'P. Rendimiento'!B9*1.1*0.9)/(B9*60)</f>
+        <v>0.99916783878090099</v>
+      </c>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="22">
-        <f>B9/B11</f>
-        <v>0.99607142857142861</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="9">
-        <f>D9*D10</f>
-        <v>1.026174256005737</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="9">
-        <f>('E.G. Equipamiento'!E5*0.97*0.9)/('E.G. Equipamiento'!E5*0.9)</f>
-        <v>0.97000000000000008</v>
-      </c>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="1">
-        <f>B11-B10</f>
-        <v>6.9725000000000001</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="9">
-        <f>('P. Rendimiento'!F5*'P. Rendimiento'!B9*1.1*0.9)/(B9*60)</f>
-        <v>1.1287916816063108</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="B10" s="1">
-        <f>99/3600</f>
-        <v>2.75E-2</v>
+        <f>8-B12</f>
+        <v>6.833333333333333</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="9">
+        <v>81</v>
+      </c>
+      <c r="D10" s="8">
         <f>1/1.1</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="11"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="1">
-        <f>8-B12</f>
-        <v>7</v>
-      </c>
+      <c r="A11" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="5">
+        <f>VSM!K10/3600</f>
+        <v>6.269907407407406E-2</v>
+      </c>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1</v>
+      <c r="A12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="5">
+        <f xml:space="preserve"> 70/60</f>
+        <v>1.1666666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G13" s="1" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="G8:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
KPIS sem y mensual entorno real
jhhj
</commit_message>
<xml_diff>
--- a/project/Documents/03. KPIs.xlsx
+++ b/project/Documents/03. KPIs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yovan\Desktop\APM\ausol-apm.github.io\project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\ausol-apm.github.io\project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3334B3F-6703-4750-B414-8807AF66BF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E36697-429B-49C3-A292-EAD83FD2EBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempos" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="147">
   <si>
     <t>Etapa</t>
   </si>
@@ -471,6 +471,15 @@
   </si>
   <si>
     <t>Total pallets (día)</t>
+  </si>
+  <si>
+    <t>Entorno</t>
+  </si>
+  <si>
+    <t>Semanal ( Max)</t>
+  </si>
+  <si>
+    <t>Mensual (Max)</t>
   </si>
 </sst>
 </file>
@@ -713,6 +722,15 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -721,15 +739,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1632,32 +1641,32 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.90625" style="1"/>
+    <col min="1" max="1" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-    </row>
-    <row r="2" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1673,12 +1682,12 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="33"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H2" s="36"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -1695,10 +1704,10 @@
         <f>C3+D3</f>
         <v>40</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1.2</v>
       </c>
@@ -1715,10 +1724,10 @@
         <f t="shared" ref="E4:E5" si="0">C4+D4</f>
         <v>40</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1.3</v>
       </c>
@@ -1735,10 +1744,10 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1755,10 +1764,10 @@
         <f t="shared" ref="E6:E17" si="1">C6+D6</f>
         <v>6</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1775,10 +1784,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>3.1</v>
       </c>
@@ -1795,10 +1804,10 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3.2</v>
       </c>
@@ -1817,7 +1826,7 @@
       </c>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>4.0999999999999996</v>
       </c>
@@ -1836,7 +1845,7 @@
       </c>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>4.2</v>
       </c>
@@ -1855,7 +1864,7 @@
       </c>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>4.3</v>
       </c>
@@ -1873,7 +1882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -1891,7 +1900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1909,7 +1918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -1927,7 +1936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -1945,7 +1954,7 @@
         <v>10.06</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -1963,7 +1972,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1972,15 +1981,15 @@
         <v>221.06</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="32" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -1994,7 +2003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -2008,7 +2017,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1.2</v>
       </c>
@@ -2022,7 +2031,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>2.1</v>
       </c>
@@ -2036,7 +2045,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2050,7 +2059,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>3.1</v>
       </c>
@@ -2064,7 +2073,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>3.2</v>
       </c>
@@ -2078,7 +2087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>4</v>
       </c>
@@ -2092,7 +2101,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>5</v>
       </c>
@@ -2106,7 +2115,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>6</v>
       </c>
@@ -2120,7 +2129,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>7</v>
       </c>
@@ -2134,7 +2143,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>8</v>
       </c>
@@ -2148,7 +2157,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>9</v>
       </c>
@@ -2162,7 +2171,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
@@ -2195,25 +2204,25 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.08984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" style="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.81640625" customWidth="1"/>
-    <col min="9" max="9" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7265625" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.90625" style="37"/>
-    <col min="14" max="14" width="7.90625" customWidth="1"/>
-    <col min="15" max="15" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.77734375" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" style="34"/>
+    <col min="14" max="14" width="7.88671875" customWidth="1"/>
+    <col min="15" max="15" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -2242,7 +2251,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>108</v>
       </c>
@@ -2270,12 +2279,12 @@
         <f>J2*$G$7</f>
         <v>45</v>
       </c>
-      <c r="L2" s="35">
+      <c r="L2" s="32">
         <f>K2*'P. Rendimiento'!$B$1/3600</f>
         <v>1.1875</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>109</v>
       </c>
@@ -2303,12 +2312,12 @@
         <f>J3*$C$13/40</f>
         <v>36.75</v>
       </c>
-      <c r="L3" s="35">
+      <c r="L3" s="32">
         <f>K3*'P. Rendimiento'!$B$1/3600</f>
         <v>0.96979166666666672</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>110</v>
       </c>
@@ -2335,12 +2344,12 @@
         <f>J4*$C$13/40</f>
         <v>27.766666666666669</v>
       </c>
-      <c r="L4" s="35">
+      <c r="L4" s="32">
         <f>K4*'P. Rendimiento'!$B$1/3600</f>
         <v>0.73273148148148148</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>111</v>
       </c>
@@ -2369,12 +2378,12 @@
         <f>J5*$G$5/$G$5</f>
         <v>15</v>
       </c>
-      <c r="L5" s="35">
+      <c r="L5" s="32">
         <f>K5*'P. Rendimiento'!$B$1/3600</f>
         <v>0.39583333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>112</v>
       </c>
@@ -2396,12 +2405,12 @@
         <f>J6*$G$5/$G$5</f>
         <v>10</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="32">
         <f>K6*'P. Rendimiento'!$B$1/3600</f>
         <v>0.2638888888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>113</v>
       </c>
@@ -2429,12 +2438,12 @@
         <f>J7*$G$5</f>
         <v>80</v>
       </c>
-      <c r="L7" s="35">
+      <c r="L7" s="32">
         <f>K7*'P. Rendimiento'!$B$1/3600</f>
         <v>2.1111111111111112</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>114</v>
       </c>
@@ -2456,12 +2465,12 @@
         <f>L8*3600/'P. Rendimiento'!B1</f>
         <v>11.2</v>
       </c>
-      <c r="L8" s="36">
+      <c r="L8" s="33">
         <f>J8*G11/3600</f>
         <v>0.29555555555555557</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>116</v>
       </c>
@@ -2486,12 +2495,12 @@
       <c r="K9" s="27">
         <v>0</v>
       </c>
-      <c r="L9" s="35">
+      <c r="L9" s="32">
         <f>K9*'P. Rendimiento'!$B$1/3600</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>117</v>
       </c>
@@ -2516,7 +2525,7 @@
         <v>225.71666666666664</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>118</v>
       </c>
@@ -2537,12 +2546,12 @@
       <c r="K11" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="L11" s="37">
+      <c r="L11" s="34">
         <f>SUM(L2:L9)</f>
         <v>5.9564120370370368</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>119</v>
       </c>
@@ -2561,7 +2570,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2570,7 +2579,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>1</v>
       </c>
@@ -2594,7 +2603,7 @@
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="24">
         <v>1</v>
       </c>
@@ -2620,7 +2629,7 @@
       <c r="J16"/>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="24">
         <v>2</v>
       </c>
@@ -2646,7 +2655,7 @@
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="24">
         <v>3</v>
       </c>
@@ -2665,7 +2674,7 @@
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24">
         <v>4</v>
       </c>
@@ -2680,15 +2689,15 @@
         <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
         <v>1.6712962962962961</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="34"/>
+      <c r="G19" s="37"/>
       <c r="I19" s="22"/>
       <c r="J19"/>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="24">
         <v>5</v>
       </c>
@@ -2703,13 +2712,13 @@
         <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
         <v>3.6944444444444446</v>
       </c>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
       <c r="I20" s="22"/>
       <c r="J20"/>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="24">
         <v>6</v>
       </c>
@@ -2724,13 +2733,13 @@
         <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
         <v>3.1666666666666665</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
       <c r="I21" s="22"/>
       <c r="J21"/>
       <c r="K21"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="24">
         <v>7</v>
       </c>
@@ -2752,7 +2761,7 @@
       <c r="J22"/>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="24">
         <v>8</v>
       </c>
@@ -2773,7 +2782,7 @@
       <c r="J23"/>
       <c r="K23"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="25">
         <v>9</v>
       </c>
@@ -2795,7 +2804,7 @@
       <c r="J24"/>
       <c r="K24"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25" s="1" t="s">
         <v>138</v>
@@ -2806,7 +2815,7 @@
       </c>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>133</v>
       </c>
@@ -2829,27 +2838,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="24.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -2859,10 +2868,10 @@
       <c r="C1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="32"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="1" t="s">
         <v>141</v>
       </c>
@@ -2872,8 +2881,14 @@
       <c r="I1" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
@@ -2902,8 +2917,14 @@
         <f>G2/8</f>
         <v>475</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K2" s="1">
+        <v>3269</v>
+      </c>
+      <c r="M2" s="1">
+        <v>6552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -2928,8 +2949,14 @@
         <f t="shared" si="0"/>
         <v>3325</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K3" s="1">
+        <v>3728</v>
+      </c>
+      <c r="M3" s="1">
+        <v>7482</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C4" s="16">
         <f>(B1*3)</f>
         <v>285</v>
@@ -2945,11 +2972,17 @@
         <v>475</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
+        <f>F4*$B$2</f>
         <v>2375</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K4" s="1">
+        <v>2333</v>
+      </c>
+      <c r="M4" s="1">
+        <v>4680</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>135</v>
       </c>
@@ -2975,14 +3008,24 @@
       <c r="H5" s="20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K5" s="1">
+        <v>9330</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M5" s="1">
+        <f>SUM(M2:M4)</f>
+        <v>18714</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G6" s="1">
         <f>G5*4</f>
         <v>38000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
@@ -3004,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -3021,7 +3064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -3039,7 +3082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -3058,7 +3101,7 @@
         <v>6.833333333333333</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -3067,7 +3110,7 @@
         <v>0.21578947368421053</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -3076,7 +3119,7 @@
         <v>278.04878048780489</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E18" s="2" t="s">
         <v>98</v>
       </c>
@@ -3085,7 +3128,7 @@
         <v>12.947368421052632</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>61</v>
       </c>
@@ -3098,7 +3141,7 @@
         <v>6.7569444444444438</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -3128,35 +3171,35 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.90625" style="1"/>
-    <col min="5" max="5" width="17.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" style="1"/>
-    <col min="7" max="7" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.88671875" style="1"/>
+    <col min="5" max="5" width="17.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1"/>
+    <col min="7" max="7" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" style="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.90625" style="1"/>
+    <col min="11" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -3188,7 +3231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -3220,7 +3263,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -3252,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
@@ -3293,7 +3336,7 @@
         <v>0.9859154929577465</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>75</v>
       </c>
@@ -3302,7 +3345,7 @@
         <v>0.87300000000000011</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>69</v>
       </c>
@@ -3323,13 +3366,13 @@
       <c r="F8" s="8">
         <v>0.97</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-    </row>
-    <row r="9" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+    </row>
+    <row r="9" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>78</v>
       </c>
@@ -3344,11 +3387,11 @@
         <f>('P. Rendimiento'!F5*'P. Rendimiento'!B9*1.1*0.9)/(B9*60)</f>
         <v>0.99916783878090099</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>76</v>
       </c>
@@ -3363,11 +3406,11 @@
         <f>1/1.1</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>99</v>
       </c>
@@ -3375,11 +3418,11 @@
         <f>VSM!K10/3600</f>
         <v>6.269907407407406E-2</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>77</v>
       </c>
@@ -3388,7 +3431,7 @@
         <v>1.1666666666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G13" s="1" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
Proyección de ventas y perfil de demanda juguetes
Excel y documento descriptivo con referencias
</commit_message>
<xml_diff>
--- a/project/Documents/03. KPIs.xlsx
+++ b/project/Documents/03. KPIs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yovan\Desktop\APM\ausol-apm.github.io\project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\ausol-apm.github.io\project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D28C2EF-1F77-4B6B-BA33-D4B747E02C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA0B5B3-B260-4566-9084-8C185A973F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempos" sheetId="2" r:id="rId1"/>
@@ -776,6 +776,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -787,12 +793,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1695,32 +1695,32 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.90625" style="1"/>
+    <col min="1" max="1" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-    </row>
-    <row r="2" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1736,12 +1736,12 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="36"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -1758,10 +1758,10 @@
         <f>C3+D3</f>
         <v>40</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1.2</v>
       </c>
@@ -1778,10 +1778,10 @@
         <f t="shared" ref="E4:E5" si="0">C4+D4</f>
         <v>40</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1.3</v>
       </c>
@@ -1798,10 +1798,10 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1818,10 +1818,10 @@
         <f t="shared" ref="E6:E17" si="1">C6+D6</f>
         <v>6</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1838,10 +1838,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>3.1</v>
       </c>
@@ -1858,10 +1858,10 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3.2</v>
       </c>
@@ -1880,7 +1880,7 @@
       </c>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>4.0999999999999996</v>
       </c>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>4.2</v>
       </c>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>4.3</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>10.06</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D18" s="1" t="s">
         <v>13</v>
       </c>
@@ -2035,15 +2035,15 @@
         <v>221.06</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="35" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1.2</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>2.1</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>3.1</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>3.2</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>4</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>5</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>6</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>7</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>8</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>9</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>10</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
@@ -2272,25 +2272,25 @@
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.08984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" style="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.81640625" customWidth="1"/>
-    <col min="9" max="9" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.81640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.90625" style="34"/>
-    <col min="14" max="14" width="7.90625" customWidth="1"/>
-    <col min="15" max="15" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.77734375" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" style="34"/>
+    <col min="14" max="14" width="7.88671875" customWidth="1"/>
+    <col min="15" max="15" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>107</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>1.1875</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>0.96979166666666672</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>109</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>0.73273148148148148</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>110</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>0.39583333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>111</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>0.2638888888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>2.1111111111111112</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>113</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>0.29555555555555557</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>115</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>1.0027777777777778</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>116</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>263.71666666666664</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>117</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>6.959189814814815</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>118</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I14" t="s">
         <v>103</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>0.155</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>1</v>
       </c>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="24">
         <v>1</v>
       </c>
@@ -2727,7 +2727,7 @@
       </c>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="24">
         <v>2</v>
       </c>
@@ -2752,7 +2752,7 @@
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="24">
         <v>3</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24">
         <v>4</v>
       </c>
@@ -2792,10 +2792,10 @@
         <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
         <v>1.6712962962962961</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="37"/>
+      <c r="G19" s="39"/>
       <c r="I19" s="22" t="s">
         <v>151</v>
       </c>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="24">
         <v>5</v>
       </c>
@@ -2820,15 +2820,15 @@
         <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
         <v>3.6944444444444446</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
       <c r="I20" s="22" t="s">
         <v>152</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="24">
         <v>6</v>
       </c>
@@ -2843,15 +2843,15 @@
         <f>Tabla4[[#This Row],[Tp (s)]]*'P. Rendimiento'!$B$1/3600</f>
         <v>3.1666666666666665</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
       <c r="I21" s="22" t="s">
         <v>153</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="24">
         <v>7</v>
       </c>
@@ -2873,7 +2873,7 @@
       <c r="J22"/>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="24">
         <v>8</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="J23"/>
       <c r="K23"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="25">
         <v>9</v>
       </c>
@@ -2916,7 +2916,7 @@
       <c r="J24"/>
       <c r="K24"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25" s="1" t="s">
         <v>136</v>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>132</v>
       </c>
@@ -2953,25 +2953,25 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="24.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -2981,10 +2981,10 @@
       <c r="C1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="35"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="1" t="s">
         <v>139</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>0.93842105263157893</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C4" s="16">
         <f>(B1*3)</f>
         <v>285</v>
@@ -3075,7 +3075,7 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>134</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F6" s="1" t="s">
         <v>147</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>38000</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>6.833333333333333</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>0.21578947368421053</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -3204,68 +3204,80 @@
         <f>60/B11</f>
         <v>278.04878048780489</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H14" s="39" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H14" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="I14" s="39" t="s">
+      <c r="I14" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="J14" s="39" t="s">
+      <c r="J14" s="35" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H15" s="39" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H15" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="39">
+      <c r="I15" s="35">
         <v>3474</v>
       </c>
-      <c r="J15" s="39">
+      <c r="J15" s="35">
         <v>14757</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H16" s="39" t="s">
+      <c r="K15" s="1">
+        <f>(J15/J18)*100</f>
+        <v>40.192286741475108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H16" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="39">
+      <c r="I16" s="35">
         <v>3033</v>
       </c>
-      <c r="J16" s="39">
+      <c r="J16" s="35">
         <v>12873</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H17" s="39" t="s">
+      <c r="K16" s="1">
+        <f>(J16/J18)*100</f>
+        <v>35.061008824490685</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H17" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="35">
         <v>2141</v>
       </c>
-      <c r="J17" s="39">
+      <c r="J17" s="35">
         <v>9086</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" s="1">
+        <f>(J17/J18)*100</f>
+        <v>24.746704434034207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E18" s="2" t="s">
         <v>98</v>
       </c>
@@ -3273,32 +3285,32 @@
         <f>C2*60*60/F5</f>
         <v>12.947368421052632</v>
       </c>
-      <c r="H18" s="39" t="s">
+      <c r="H18" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="39">
+      <c r="I18" s="35">
         <f>SUM(I15:I17)</f>
         <v>8648</v>
       </c>
-      <c r="J18" s="39">
+      <c r="J18" s="35">
         <f>SUM(J15:J17)</f>
         <v>36716</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H19" s="39" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H19" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="I19" s="40">
+      <c r="I19" s="36">
         <f>1-I18/G5</f>
         <v>8.9684210526315811E-2</v>
       </c>
-      <c r="J19" s="40">
+      <c r="J19" s="36">
         <f>1-J18/G6</f>
         <v>3.378947368421048E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>61</v>
       </c>
@@ -3311,7 +3323,7 @@
         <v>6.7569444444444438</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -3323,7 +3335,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H22" s="1" t="s">
         <v>145</v>
       </c>
@@ -3331,7 +3343,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H23" s="1" t="s">
         <v>13</v>
       </c>
@@ -3359,35 +3371,35 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.90625" style="1"/>
-    <col min="5" max="5" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.88671875" style="1"/>
+    <col min="5" max="5" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" style="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.90625" style="1"/>
+    <col min="11" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -3419,7 +3431,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -3451,7 +3463,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -3483,7 +3495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
@@ -3524,7 +3536,7 @@
         <v>0.99270072992700731</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>75</v>
       </c>
@@ -3533,7 +3545,7 @@
         <v>0.82755980861244005</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>69</v>
       </c>
@@ -3549,7 +3561,7 @@
         <v>1.0819845243897019</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>78</v>
       </c>
@@ -3565,7 +3577,7 @@
         <v>1.1901829768286722</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>76</v>
       </c>
@@ -3581,7 +3593,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>99</v>
       </c>
@@ -3597,7 +3609,7 @@
         <v>0.97005047672462141</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>77</v>
       </c>
@@ -3606,7 +3618,7 @@
         <v>1.1666666666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G13" s="1" t="s">
         <v>92</v>
       </c>

</xml_diff>